<commit_message>
New moments, graphs and descriptive statistics
</commit_message>
<xml_diff>
--- a/Code/Descriptives.xlsx
+++ b/Code/Descriptives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5604ff08deb8de49/Documents/Research/Denmark/IncomeUncertaintyGit/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE746DD9-362F-4482-9958-92F9D0611380}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCBD9F7A-9741-4897-83C7-28F0C602FA89}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
   <si>
     <t>inc</t>
   </si>
@@ -103,138 +103,15 @@
     <t>-------------+--------------------------------------------------------------------------------</t>
   </si>
   <si>
-    <t>59296.25</t>
-  </si>
-  <si>
-    <t>28815.54</t>
-  </si>
-  <si>
-    <t>25241.4</t>
-  </si>
-  <si>
-    <t>34645.76</t>
-  </si>
-  <si>
-    <t>57867.36</t>
-  </si>
-  <si>
-    <t>78779.93</t>
-  </si>
-  <si>
-    <t>95291.77</t>
-  </si>
-  <si>
-    <t>52704.29</t>
-  </si>
-  <si>
-    <t>28579.66</t>
-  </si>
-  <si>
-    <t>22266.9</t>
-  </si>
-  <si>
-    <t>30438.57</t>
-  </si>
-  <si>
-    <t>48378.25</t>
-  </si>
-  <si>
-    <t>68240.1</t>
-  </si>
-  <si>
-    <t>88623.27</t>
-  </si>
-  <si>
     <t>liquidasse~j</t>
   </si>
   <si>
-    <t>18458.52</t>
-  </si>
-  <si>
-    <t>33033.26</t>
-  </si>
-  <si>
-    <t>20520.99</t>
-  </si>
-  <si>
-    <t>47943.63</t>
-  </si>
-  <si>
     <t>netwealth_~j</t>
   </si>
   <si>
-    <t>75045.1</t>
-  </si>
-  <si>
-    <t>157357.8</t>
-  </si>
-  <si>
-    <t>-44664.11</t>
-  </si>
-  <si>
-    <t>-10199.27</t>
-  </si>
-  <si>
-    <t>19270.79</t>
-  </si>
-  <si>
-    <t>128065.2</t>
-  </si>
-  <si>
-    <t>260826.3</t>
-  </si>
-  <si>
-    <t>.567613</t>
-  </si>
-  <si>
-    <t>.4954074</t>
-  </si>
-  <si>
-    <t>.6589255</t>
-  </si>
-  <si>
-    <t>.4740704</t>
-  </si>
-  <si>
-    <t>.3107731</t>
-  </si>
-  <si>
-    <t>.4628101</t>
-  </si>
-  <si>
     <t>alder_hea~08</t>
   </si>
   <si>
-    <t>-28052.77</t>
-  </si>
-  <si>
-    <t>-59148.33</t>
-  </si>
-  <si>
-    <t>-12626.23</t>
-  </si>
-  <si>
-    <t>39376.46</t>
-  </si>
-  <si>
-    <t>-109693.5</t>
-  </si>
-  <si>
-    <t>156529.7</t>
-  </si>
-  <si>
-    <t>-303864.9</t>
-  </si>
-  <si>
-    <t>-193930.2</t>
-  </si>
-  <si>
-    <t>-65824.98</t>
-  </si>
-  <si>
-    <t>14515.76</t>
-  </si>
-  <si>
     <t>----------------------------------------------------------------------------------------------</t>
   </si>
   <si>
@@ -253,18 +130,6 @@
     <t>53303.79</t>
   </si>
   <si>
-    <t>1.46e+07</t>
-  </si>
-  <si>
-    <t>49252.33</t>
-  </si>
-  <si>
-    <t>26487.17</t>
-  </si>
-  <si>
-    <t>45214.61</t>
-  </si>
-  <si>
     <t>23331.43</t>
   </si>
   <si>
@@ -337,18 +202,6 @@
     <t>36578.59</t>
   </si>
   <si>
-    <t>3.28e+07</t>
-  </si>
-  <si>
-    <t>40921.53</t>
-  </si>
-  <si>
-    <t>25269.83</t>
-  </si>
-  <si>
-    <t>34326.1</t>
-  </si>
-  <si>
     <t>24855.52</t>
   </si>
   <si>
@@ -463,7 +316,163 @@
     <t>Number of household-year observations</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: Values are 2015 USD. Age refers to the age in 2008 of the main income earner in the household. For the purposes of calculation of consumption in the population, top and bottom 5% in terms of consumption have been excluded. URE and NNP can only be calculated in the period 2009-2015 due to mortgage information being insufficiently detailed in the previous years. </t>
+    <t>1.55e+07</t>
+  </si>
+  <si>
+    <t>51427.49</t>
+  </si>
+  <si>
+    <t>43311.74</t>
+  </si>
+  <si>
+    <t>45222.23</t>
+  </si>
+  <si>
+    <t>3.45e+07</t>
+  </si>
+  <si>
+    <t>42261.84</t>
+  </si>
+  <si>
+    <t>39336.87</t>
+  </si>
+  <si>
+    <t>33965.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Values are 2015 USD. Age refers to the age in 2008 of the main income earner in the household. For the purposes of calculation of consumption in the population, top and bottom 1% in terms of consumption have been excluded. URE and NNP can only be calculated in the period 2009-2015 due to mortgage information being insufficiently detailed in the previous years. </t>
+  </si>
+  <si>
+    <t>59261.43</t>
+  </si>
+  <si>
+    <t>28819.4</t>
+  </si>
+  <si>
+    <t>25223.8</t>
+  </si>
+  <si>
+    <t>34614.81</t>
+  </si>
+  <si>
+    <t>57804.09</t>
+  </si>
+  <si>
+    <t>78754.18</t>
+  </si>
+  <si>
+    <t>95269.59</t>
+  </si>
+  <si>
+    <t>52680.2</t>
+  </si>
+  <si>
+    <t>28581.18</t>
+  </si>
+  <si>
+    <t>22252.98</t>
+  </si>
+  <si>
+    <t>30416.9</t>
+  </si>
+  <si>
+    <t>48344.13</t>
+  </si>
+  <si>
+    <t>68215.79</t>
+  </si>
+  <si>
+    <t>88603.07</t>
+  </si>
+  <si>
+    <t>18437.72</t>
+  </si>
+  <si>
+    <t>33015.97</t>
+  </si>
+  <si>
+    <t>20489.76</t>
+  </si>
+  <si>
+    <t>47894.74</t>
+  </si>
+  <si>
+    <t>74937.47</t>
+  </si>
+  <si>
+    <t>157295.3</t>
+  </si>
+  <si>
+    <t>-44649.34</t>
+  </si>
+  <si>
+    <t>-10229.63</t>
+  </si>
+  <si>
+    <t>19114.52</t>
+  </si>
+  <si>
+    <t>127879.7</t>
+  </si>
+  <si>
+    <t>260625.4</t>
+  </si>
+  <si>
+    <t>.5668571</t>
+  </si>
+  <si>
+    <t>.49551</t>
+  </si>
+  <si>
+    <t>.6583733</t>
+  </si>
+  <si>
+    <t>.4742551</t>
+  </si>
+  <si>
+    <t>.3105533</t>
+  </si>
+  <si>
+    <t>.4627202</t>
+  </si>
+  <si>
+    <t>-47912.78</t>
+  </si>
+  <si>
+    <t>130967.2</t>
+  </si>
+  <si>
+    <t>-184936.6</t>
+  </si>
+  <si>
+    <t>-82530.16</t>
+  </si>
+  <si>
+    <t>-16164.02</t>
+  </si>
+  <si>
+    <t>5252.54</t>
+  </si>
+  <si>
+    <t>36753.89</t>
+  </si>
+  <si>
+    <t>-109685.2</t>
+  </si>
+  <si>
+    <t>156523.2</t>
+  </si>
+  <si>
+    <t>-303845.5</t>
+  </si>
+  <si>
+    <t>-193918.6</t>
+  </si>
+  <si>
+    <t>-65809.63</t>
+  </si>
+  <si>
+    <t>14514.62</t>
   </si>
 </sst>
 </file>
@@ -895,7 +904,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -906,7 +915,7 @@
     <col min="4" max="4" width="8.5234375" customWidth="1"/>
     <col min="5" max="5" width="9.20703125" customWidth="1"/>
     <col min="6" max="6" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5234375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.20703125" customWidth="1"/>
     <col min="10" max="10" width="9.5234375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5234375" bestFit="1" customWidth="1"/>
@@ -968,28 +977,28 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1000,92 +1009,92 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5">
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="G5" s="7">
-        <v>884.13900000000001</v>
+        <v>880.54470000000003</v>
       </c>
       <c r="H5" s="2">
-        <v>2350.2809999999999</v>
+        <v>2344.5619999999999</v>
       </c>
       <c r="I5" s="2">
-        <v>6870.0680000000002</v>
+        <v>6855.7179999999998</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6">
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1096,13 +1105,13 @@
         <v>11</v>
       </c>
       <c r="D7">
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1128,13 +1137,13 @@
         <v>11</v>
       </c>
       <c r="D8">
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1160,13 +1169,13 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>7531530</v>
+        <v>7545899</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1186,19 +1195,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10">
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="E10" s="2">
-        <v>43.54007</v>
+        <v>43.537370000000003</v>
       </c>
       <c r="F10" s="2">
-        <v>7.1069149999999999</v>
+        <v>7.1081950000000003</v>
       </c>
       <c r="G10">
         <v>33</v>
@@ -1224,28 +1233,28 @@
         <v>11</v>
       </c>
       <c r="D11">
-        <v>4815078</v>
+        <v>4815908</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11">
-        <v>108390</v>
-      </c>
-      <c r="G11">
-        <v>-120372</v>
+        <v>129</v>
+      </c>
+      <c r="F11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="2">
-        <v>6856.9970000000003</v>
+        <v>133</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="K11" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1256,33 +1265,33 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>4815078</v>
+        <v>4815908</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
       <c r="I12" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="J12" s="2">
-        <v>-3232.7089999999998</v>
+        <v>-3232.931</v>
       </c>
       <c r="K12" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1310,7 +1319,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1321,16 +1330,16 @@
         <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1341,58 +1350,58 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2">
-        <v>6577694</v>
+        <v>6577.6940000000004</v>
       </c>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1403,13 +1412,13 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1423,13 +1432,13 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1443,13 +1452,13 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1457,13 +1466,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2">
         <v>42.460659999999997</v>
@@ -1486,13 +1495,13 @@
         <v>9009302</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1506,18 +1515,18 @@
         <v>9026373</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1542,7 +1551,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1553,16 +1562,16 @@
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="G32" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1573,33 +1582,33 @@
         <v>11</v>
       </c>
       <c r="D33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E33" t="s">
-        <v>97</v>
-      </c>
-      <c r="F33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="G34" s="2">
         <v>6621.3969999999999</v>
@@ -1607,22 +1616,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="F35">
         <v>1099427</v>
       </c>
       <c r="G35" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1633,13 +1642,13 @@
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="F36" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1653,13 +1662,13 @@
         <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="F37" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -1673,13 +1682,13 @@
         <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="E38" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="F38" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1687,13 +1696,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="E39" s="2">
         <v>49.016779999999997</v>
@@ -1713,10 +1722,10 @@
         <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="F40">
         <v>269370</v>
@@ -1733,21 +1742,21 @@
         <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="E41" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="F41" s="2">
         <v>481950</v>
       </c>
       <c r="G41" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1760,7 +1769,7 @@
   <dimension ref="A2:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:P15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1784,7 +1793,7 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>134</v>
+        <v>85</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -1794,13 +1803,13 @@
       <c r="H2" s="10"/>
       <c r="I2" s="3"/>
       <c r="J2" s="10" t="s">
-        <v>135</v>
+        <v>86</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="3"/>
       <c r="N2" s="10" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
@@ -1808,78 +1817,78 @@
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9">
         <f>'Ark1'!E3*1</f>
-        <v>59296.25</v>
+        <v>59261.43</v>
       </c>
       <c r="C4" s="9">
         <f>'Ark1'!F3*1</f>
-        <v>28815.54</v>
+        <v>28819.4</v>
       </c>
       <c r="D4" s="9">
         <f>'Ark1'!G3*1</f>
-        <v>25241.4</v>
+        <v>25223.8</v>
       </c>
       <c r="E4" s="9">
         <f>'Ark1'!H3*1</f>
-        <v>34645.760000000002</v>
+        <v>34614.81</v>
       </c>
       <c r="F4" s="9">
         <f>'Ark1'!I3*1</f>
-        <v>57867.360000000001</v>
+        <v>57804.09</v>
       </c>
       <c r="G4" s="9">
         <f>'Ark1'!J3*1</f>
-        <v>78779.929999999993</v>
+        <v>78754.179999999993</v>
       </c>
       <c r="H4" s="9">
         <f>'Ark1'!K3*1</f>
-        <v>95291.77</v>
+        <v>95269.59</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9">
@@ -1910,94 +1919,94 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="B5" s="9">
         <f>'Ark1'!E4*1</f>
-        <v>52704.29</v>
+        <v>52680.2</v>
       </c>
       <c r="C5" s="9">
         <f>'Ark1'!F4*1</f>
-        <v>28579.66</v>
+        <v>28581.18</v>
       </c>
       <c r="D5" s="9">
         <f>'Ark1'!G4*1</f>
-        <v>22266.9</v>
+        <v>22252.98</v>
       </c>
       <c r="E5" s="9">
         <f>'Ark1'!H4*1</f>
-        <v>30438.57</v>
+        <v>30416.9</v>
       </c>
       <c r="F5" s="9">
         <f>'Ark1'!I4*1</f>
-        <v>48378.25</v>
+        <v>48344.13</v>
       </c>
       <c r="G5" s="9">
         <f>'Ark1'!J4*1</f>
-        <v>68240.100000000006</v>
+        <v>68215.789999999994</v>
       </c>
       <c r="H5" s="9">
         <f>'Ark1'!K4*1</f>
-        <v>88623.27</v>
+        <v>88603.07</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9">
         <f>'Ark1'!E19*1</f>
-        <v>49252.33</v>
+        <v>51427.49</v>
       </c>
       <c r="K5" s="9">
         <f>'Ark1'!F19*1</f>
-        <v>26487.17</v>
+        <v>43311.74</v>
       </c>
       <c r="L5" s="9">
         <f>'Ark1'!G19*1</f>
-        <v>45214.61</v>
+        <v>45222.23</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9">
         <f>'Ark1'!E33*1</f>
-        <v>40921.53</v>
+        <v>42261.84</v>
       </c>
       <c r="O5" s="9">
         <f>'Ark1'!F33*1</f>
-        <v>25269.83</v>
+        <v>39336.870000000003</v>
       </c>
       <c r="P5" s="9">
         <f>'Ark1'!G33*1</f>
-        <v>34326.1</v>
+        <v>33965.72</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="B6" s="9">
         <f>'Ark1'!E5*1</f>
-        <v>18458.52</v>
+        <v>18437.72</v>
       </c>
       <c r="C6" s="9">
         <f>'Ark1'!F5*1</f>
-        <v>33033.26</v>
+        <v>33015.97</v>
       </c>
       <c r="D6" s="9">
         <f>'Ark1'!G5*1</f>
-        <v>884.13900000000001</v>
+        <v>880.54470000000003</v>
       </c>
       <c r="E6" s="9">
         <f>'Ark1'!H5*1</f>
-        <v>2350.2809999999999</v>
+        <v>2344.5619999999999</v>
       </c>
       <c r="F6" s="9">
         <f>'Ark1'!I5*1</f>
-        <v>6870.0680000000002</v>
+        <v>6855.7179999999998</v>
       </c>
       <c r="G6" s="9">
         <f>'Ark1'!J5*1</f>
-        <v>20520.990000000002</v>
+        <v>20489.759999999998</v>
       </c>
       <c r="H6" s="9">
         <f>'Ark1'!K5*1</f>
-        <v>47943.63</v>
+        <v>47894.74</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9">
@@ -2010,7 +2019,7 @@
       </c>
       <c r="L6" s="9">
         <f>'Ark1'!G20*1</f>
-        <v>6577694</v>
+        <v>6577.6940000000004</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9">
@@ -2028,35 +2037,35 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B7" s="9">
         <f>'Ark1'!E6*1</f>
-        <v>75045.100000000006</v>
+        <v>74937.47</v>
       </c>
       <c r="C7" s="9">
         <f>'Ark1'!F6*1</f>
-        <v>157357.79999999999</v>
+        <v>157295.29999999999</v>
       </c>
       <c r="D7" s="9">
         <f>'Ark1'!G6*1</f>
-        <v>-44664.11</v>
+        <v>-44649.34</v>
       </c>
       <c r="E7" s="9">
         <f>'Ark1'!H6*1</f>
-        <v>-10199.27</v>
+        <v>-10229.629999999999</v>
       </c>
       <c r="F7" s="9">
         <f>'Ark1'!I6*1</f>
-        <v>19270.79</v>
+        <v>19114.52</v>
       </c>
       <c r="G7" s="9">
         <f>'Ark1'!J6*1</f>
-        <v>128065.2</v>
+        <v>127879.7</v>
       </c>
       <c r="H7" s="9">
         <f>'Ark1'!K6*1</f>
-        <v>260826.3</v>
+        <v>260625.4</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9">
@@ -2087,15 +2096,15 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="B8" s="8">
         <f>'Ark1'!E7*1</f>
-        <v>0.56761300000000003</v>
+        <v>0.5668571</v>
       </c>
       <c r="C8" s="8">
         <f>'Ark1'!F7*1</f>
-        <v>0.4954074</v>
+        <v>0.49551000000000001</v>
       </c>
       <c r="D8" s="8">
         <f>'Ark1'!G7*1</f>
@@ -2146,15 +2155,15 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="B9" s="8">
         <f>'Ark1'!E8*1</f>
-        <v>0.65892550000000005</v>
+        <v>0.65837330000000005</v>
       </c>
       <c r="C9" s="8">
         <f>'Ark1'!F8*1</f>
-        <v>0.4740704</v>
+        <v>0.47425509999999999</v>
       </c>
       <c r="D9" s="8">
         <f>'Ark1'!G8*1</f>
@@ -2205,15 +2214,15 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="B10" s="8">
         <f>'Ark1'!E9*1</f>
-        <v>0.31077310000000002</v>
+        <v>0.31055329999999998</v>
       </c>
       <c r="C10" s="8">
         <f>'Ark1'!F9*1</f>
-        <v>0.4628101</v>
+        <v>0.46272020000000003</v>
       </c>
       <c r="D10" s="8">
         <f>'Ark1'!G9*1</f>
@@ -2264,15 +2273,15 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="B11" s="9">
         <f>'Ark1'!E10*1</f>
-        <v>43.54007</v>
+        <v>43.537370000000003</v>
       </c>
       <c r="C11" s="9">
         <f>'Ark1'!F10*1</f>
-        <v>7.1069149999999999</v>
+        <v>7.1081950000000003</v>
       </c>
       <c r="D11" s="9">
         <f>'Ark1'!G10*1</f>
@@ -2323,35 +2332,35 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="B12" s="9">
         <f>'Ark1'!E11*1</f>
-        <v>-28052.77</v>
+        <v>-47912.78</v>
       </c>
       <c r="C12" s="9">
         <f>'Ark1'!F11*1</f>
-        <v>108390</v>
+        <v>130967.2</v>
       </c>
       <c r="D12" s="9">
         <f>'Ark1'!G11*1</f>
-        <v>-120372</v>
+        <v>-184936.6</v>
       </c>
       <c r="E12" s="9">
         <f>'Ark1'!H11*1</f>
-        <v>-59148.33</v>
+        <v>-82530.16</v>
       </c>
       <c r="F12" s="9">
         <f>'Ark1'!I11*1</f>
-        <v>-12626.23</v>
+        <v>-16164.02</v>
       </c>
       <c r="G12" s="9">
         <f>'Ark1'!J11*1</f>
-        <v>6856.9970000000003</v>
+        <v>5252.54</v>
       </c>
       <c r="H12" s="9">
         <f>'Ark1'!K11*1</f>
-        <v>39376.46</v>
+        <v>36753.89</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9">
@@ -2382,35 +2391,35 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="B13" s="9">
         <f>'Ark1'!E12*1</f>
-        <v>-109693.5</v>
+        <v>-109685.2</v>
       </c>
       <c r="C13" s="9">
         <f>'Ark1'!F12*1</f>
-        <v>156529.70000000001</v>
+        <v>156523.20000000001</v>
       </c>
       <c r="D13" s="9">
         <f>'Ark1'!G12*1</f>
-        <v>-303864.90000000002</v>
+        <v>-303845.5</v>
       </c>
       <c r="E13" s="9">
         <f>'Ark1'!H12*1</f>
-        <v>-193930.2</v>
+        <v>-193918.6</v>
       </c>
       <c r="F13" s="9">
         <f>'Ark1'!I12*1</f>
-        <v>-65824.98</v>
+        <v>-65809.63</v>
       </c>
       <c r="G13" s="9">
         <f>'Ark1'!J12*1</f>
-        <v>-3232.7089999999998</v>
+        <v>-3232.931</v>
       </c>
       <c r="H13" s="9">
         <f>'Ark1'!K12*1</f>
-        <v>14515.76</v>
+        <v>14514.62</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9">
@@ -2441,11 +2450,11 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="B14" s="6">
         <f>'Ark1'!D3*1</f>
-        <v>7649501</v>
+        <v>7664360</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2468,7 +2477,7 @@
     </row>
     <row r="15" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>

</xml_diff>

<commit_message>
Write up of results by liquid and net wealth
</commit_message>
<xml_diff>
--- a/Code/Descriptives.xlsx
+++ b/Code/Descriptives.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5604ff08deb8de49/Documents/Research/Denmark/IncomeUncertaintyGit/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmun\OneDrive\Documents\Research\Denmark\IncomeUncertaintyGit\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C36610-5F41-4E46-B321-3FEAF74056C2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B61EBF88-025B-4474-B984-65676F19AC07}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1768,7 +1768,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>

</xml_diff>

<commit_message>
Massive update to all graphs following changes to URE definitions
</commit_message>
<xml_diff>
--- a/Code/Descriptives.xlsx
+++ b/Code/Descriptives.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmun\OneDrive\Documents\Research\Denmark\IncomeUncertaintyGit\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B61EBF88-025B-4474-B984-65676F19AC07}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57E37AC2-20EB-41DA-8978-EDCFDB180F4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
   <si>
     <t>inc</t>
   </si>
@@ -229,9 +229,6 @@
     <t>3.95e+07</t>
   </si>
   <si>
-    <t>2.02e+07</t>
-  </si>
-  <si>
     <t>2.03e+07</t>
   </si>
   <si>
@@ -304,33 +301,6 @@
     <t>Number of household-year observations</t>
   </si>
   <si>
-    <t>1.55e+07</t>
-  </si>
-  <si>
-    <t>51427.49</t>
-  </si>
-  <si>
-    <t>43311.74</t>
-  </si>
-  <si>
-    <t>45222.23</t>
-  </si>
-  <si>
-    <t>3.45e+07</t>
-  </si>
-  <si>
-    <t>42261.84</t>
-  </si>
-  <si>
-    <t>39336.87</t>
-  </si>
-  <si>
-    <t>33965.72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: Values are 2015 USD. Age refers to the age in 2008 of the main income earner in the household. For the purposes of calculation of consumption in the population, top and bottom 1% in terms of consumption have been excluded. URE and NNP can only be calculated in the period 2009-2015 due to mortgage information being insufficiently detailed in the previous years. </t>
-  </si>
-  <si>
     <t>59261.43</t>
   </si>
   <si>
@@ -463,16 +433,49 @@
     <t>39371.09</t>
   </si>
   <si>
-    <t>-44134.45</t>
-  </si>
-  <si>
-    <t>245654.7</t>
-  </si>
-  <si>
-    <t>-18394.63</t>
-  </si>
-  <si>
-    <t>-20259.4</t>
+    <t>1.39e+07</t>
+  </si>
+  <si>
+    <t>54022.09</t>
+  </si>
+  <si>
+    <t>38126.09</t>
+  </si>
+  <si>
+    <t>46373.22</t>
+  </si>
+  <si>
+    <t>-47588.8</t>
+  </si>
+  <si>
+    <t>243604.3</t>
+  </si>
+  <si>
+    <t>-19374.19</t>
+  </si>
+  <si>
+    <t>3.14e+07</t>
+  </si>
+  <si>
+    <t>44225.26</t>
+  </si>
+  <si>
+    <t>35040.87</t>
+  </si>
+  <si>
+    <t>34655.73</t>
+  </si>
+  <si>
+    <t>1.93e+07</t>
+  </si>
+  <si>
+    <t>-24172.06</t>
+  </si>
+  <si>
+    <t>210497.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Values are 2015 USD. Age refers to the age in 2008 of the main income earner in the household. For the purposes of calculation of consumption in the population, top 1% and negative values of consumption have been excluded. URE and NNP can only be calculated in the period 2009-2015 due to mortgage information being insufficiently detailed in the previous years. </t>
   </si>
 </sst>
 </file>
@@ -904,7 +907,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -980,25 +983,25 @@
         <v>7664360</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1012,25 +1015,25 @@
         <v>7664360</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1044,10 +1047,10 @@
         <v>7664360</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G5" s="7">
         <v>880.54470000000003</v>
@@ -1059,10 +1062,10 @@
         <v>6855.7179999999998</v>
       </c>
       <c r="J5" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1076,25 +1079,25 @@
         <v>7664360</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="H6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I6" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J6" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="K6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1108,10 +1111,10 @@
         <v>7664360</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1140,10 +1143,10 @@
         <v>7664360</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1172,10 +1175,10 @@
         <v>7545899</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1236,25 +1239,25 @@
         <v>4815908</v>
       </c>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="H11" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="K11" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1268,25 +1271,25 @@
         <v>4815908</v>
       </c>
       <c r="E12" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G12" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="H12" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="I12" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J12" s="2">
         <v>-3232.931</v>
       </c>
       <c r="K12" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1350,16 +1353,16 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="G19" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="J19" s="2"/>
     </row>
@@ -1492,16 +1495,16 @@
         <v>11</v>
       </c>
       <c r="D26">
-        <v>9009302</v>
+        <v>8503394</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F26" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G26" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1582,16 +1585,16 @@
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>136</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1722,16 +1725,16 @@
         <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="E40" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" t="s">
         <v>141</v>
       </c>
-      <c r="F40">
-        <v>256276</v>
-      </c>
       <c r="G40" s="2">
-        <v>-3041.5970000000002</v>
+        <v>-4056.5340000000001</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1742,16 +1745,16 @@
         <v>11</v>
       </c>
       <c r="D41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" t="s">
         <v>61</v>
-      </c>
-      <c r="E41" t="s">
-        <v>62</v>
       </c>
       <c r="F41" s="2">
         <v>481950</v>
       </c>
       <c r="G41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1769,7 +1772,7 @@
   <dimension ref="A2:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1793,7 +1796,7 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -1803,13 +1806,13 @@
       <c r="H2" s="10"/>
       <c r="I2" s="3"/>
       <c r="J2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="3"/>
       <c r="N2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
@@ -1817,50 +1820,50 @@
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="L3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="P3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9">
         <f>'Ark1'!E3*1</f>
@@ -1919,7 +1922,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="9">
         <f>'Ark1'!E4*1</f>
@@ -1952,33 +1955,33 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9">
         <f>'Ark1'!E19*1</f>
-        <v>51427.49</v>
+        <v>54022.09</v>
       </c>
       <c r="K5" s="9">
         <f>'Ark1'!F19*1</f>
-        <v>43311.74</v>
+        <v>38126.089999999997</v>
       </c>
       <c r="L5" s="9">
         <f>'Ark1'!G19*1</f>
-        <v>45222.23</v>
+        <v>46373.22</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9">
         <f>'Ark1'!E33*1</f>
-        <v>42261.84</v>
+        <v>44225.26</v>
       </c>
       <c r="O5" s="9">
         <f>'Ark1'!F33*1</f>
-        <v>39336.870000000003</v>
+        <v>35040.870000000003</v>
       </c>
       <c r="P5" s="9">
         <f>'Ark1'!G33*1</f>
-        <v>33965.72</v>
+        <v>34655.730000000003</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="9">
         <f>'Ark1'!E5*1</f>
@@ -2037,7 +2040,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="9">
         <f>'Ark1'!E6*1</f>
@@ -2096,7 +2099,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="8">
         <f>'Ark1'!E7*1</f>
@@ -2155,7 +2158,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="8">
         <f>'Ark1'!E8*1</f>
@@ -2214,7 +2217,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="8">
         <f>'Ark1'!E9*1</f>
@@ -2273,7 +2276,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="9">
         <f>'Ark1'!E10*1</f>
@@ -2332,7 +2335,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="9">
         <f>'Ark1'!E11*1</f>
@@ -2365,33 +2368,33 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9">
         <f>'Ark1'!E26*1</f>
-        <v>-44134.45</v>
+        <v>-47588.800000000003</v>
       </c>
       <c r="K12" s="9">
         <f>'Ark1'!F26*1</f>
-        <v>245654.7</v>
+        <v>243604.3</v>
       </c>
       <c r="L12" s="9">
         <f>'Ark1'!G26*1</f>
-        <v>-18394.63</v>
+        <v>-19374.189999999999</v>
       </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9">
         <f>'Ark1'!E40*1</f>
-        <v>-20259.400000000001</v>
+        <v>-24172.06</v>
       </c>
       <c r="O12" s="9">
         <f>'Ark1'!F40*1</f>
-        <v>256276</v>
+        <v>210497.2</v>
       </c>
       <c r="P12" s="9">
         <f>'Ark1'!G40*1</f>
-        <v>-3041.5970000000002</v>
+        <v>-4056.5340000000001</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="9">
         <f>'Ark1'!E12*1</f>
@@ -2450,7 +2453,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="6">
         <f>'Ark1'!D3*1</f>
@@ -2477,7 +2480,7 @@
     </row>
     <row r="15" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>

</xml_diff>